<commit_message>
Updates: Soil module has been replaced by a new soil module
</commit_message>
<xml_diff>
--- a/v3-0-OOP-operational/User_Inputs.xlsx
+++ b/v3-0-OOP-operational/User_Inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Diane_lab\simple_model\generic_crop_model_project\Git_OOD\Generic-Object-Oriented-Plant-Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Diane_lab\simple_model\generic_crop_model_project\Git_OOD\Generic-Object-Oriented-Plant-Model\v3-0-OOP-operational\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B25D28-BC3A-4E49-AC02-9852BCAF6A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41046424-205D-4BBC-859E-A757E54C8265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{6CB13956-ACFD-45EF-A623-5DC9742C36B6}"/>
   </bookViews>
@@ -231,12 +231,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -279,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -292,6 +298,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,8 +637,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1001,11 +1009,11 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B46">
-        <v>60</v>
+      <c r="B46" s="7">
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">

</xml_diff>